<commit_message>
add berlin 2023 election and government
</commit_message>
<xml_diff>
--- a/inst/extdata/agwatchlink.xlsx
+++ b/inst/extdata/agwatchlink.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="11113"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10409"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertstelzle/git_projekte/add_nds21/bundeslaendeR/inst/extdata/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/robertstelzle/git_projekte/bundeslaendeR/inst/extdata/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{278BC4EE-2C0E-2A4A-AB98-CAEA63CA5CD1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{29CEBA2E-E336-DC41-B2D9-C193F54A1A2E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="880" windowWidth="36000" windowHeight="21240" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1257" uniqueCount="398">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1365" uniqueCount="435">
   <si>
     <t>state</t>
   </si>
@@ -1219,6 +1219,117 @@
   </si>
   <si>
     <t>https://www.abgeordnetenwatch.de/sites/default/files/election-program-files/voltniedersachsenltw22wahlprogramm.pdf</t>
+  </si>
+  <si>
+    <t>https://www.abgeordnetenwatch.de/sites/default/files/election-program-files/spdwahlprogrammltwbln20210.pdf</t>
+  </si>
+  <si>
+    <t>https://www.abgeordnetenwatch.de/sites/default/files/election-program-files/cduwahlprogrammahw2021_0.pdf</t>
+  </si>
+  <si>
+    <t>https://www.abgeordnetenwatch.de/sites/default/files/election-program-files/bundnis90-diegrunenwahlprogrammagh2023.pdf</t>
+  </si>
+  <si>
+    <t>https://www.abgeordnetenwatch.de/sites/default/files/election-program-files/dielinkewahlprogrammberlin2023.pdf</t>
+  </si>
+  <si>
+    <t>https://www.abgeordnetenwatch.de/sites/default/files/election-program-files/afd-lvblnwahlprogramm-2023web-1.pdf</t>
+  </si>
+  <si>
+    <t>https://www.abgeordnetenwatch.de/sites/default/files/election-program-files/wahlprogramm-der-fdp-berlin-zur-abgeordnetenhauswahl-2023.pdf</t>
+  </si>
+  <si>
+    <t>https://www.abgeordnetenwatch.de/sites/default/files/election-program-files/bergparteiwahlprogramm.pdf</t>
+  </si>
+  <si>
+    <t>Bergpartei</t>
+  </si>
+  <si>
+    <t>https://www.abgeordnetenwatch.de/sites/default/files/election-program-files/bildetberlinwahlprogramm.pdf</t>
+  </si>
+  <si>
+    <t>BildetBerlin</t>
+  </si>
+  <si>
+    <t>https://www.abgeordnetenwatch.de/sites/default/files/election-program-files/die-pinkengrundsatzprogramm.pdf</t>
+  </si>
+  <si>
+    <t>PinkeBündnis21</t>
+  </si>
+  <si>
+    <t>https://www.abgeordnetenwatch.de/sites/default/files/election-program-files/dkgrundsatzprogramm.pdf</t>
+  </si>
+  <si>
+    <t>DKons</t>
+  </si>
+  <si>
+    <t>https://www.abgeordnetenwatch.de/sites/default/files/election-program-files/diebasiswahlprogramm.pdf</t>
+  </si>
+  <si>
+    <t>https://www.abgeordnetenwatch.de/sites/default/files/election-program-files/humanistenwahlprogrammahw2023.pdf</t>
+  </si>
+  <si>
+    <t>NeueDemokraten</t>
+  </si>
+  <si>
+    <t>https://www.abgeordnetenwatch.de/sites/default/files/election-program-files/neuedemokratengrundsatzprogramm.pdf</t>
+  </si>
+  <si>
+    <t>https://www.abgeordnetenwatch.de/sites/default/files/election-program-files/die-parteiwahlprogramm.pdf</t>
+  </si>
+  <si>
+    <t>https://www.abgeordnetenwatch.de/sites/default/files/election-program-files/dieurbaneparteiprogramm.pdf</t>
+  </si>
+  <si>
+    <t>Urbane</t>
+  </si>
+  <si>
+    <t>https://www.abgeordnetenwatch.de/sites/default/files/election-program-files/dkpwahlprogrammahw2023.pdf</t>
+  </si>
+  <si>
+    <t>https://www.abgeordnetenwatch.de/sites/default/files/election-program-files/20210811fwberlinwahlprogramm2023.pdf</t>
+  </si>
+  <si>
+    <t>https://www.abgeordnetenwatch.de/sites/default/files/election-program-files/klimalisteberlinwahlprogrammltwbln2023.pdf</t>
+  </si>
+  <si>
+    <t>https://www.abgeordnetenwatch.de/sites/default/files/election-program-files/menschliche-weltwahlprogramm.pdf</t>
+  </si>
+  <si>
+    <t>MenschlWelt</t>
+  </si>
+  <si>
+    <t>https://www.abgeordnetenwatch.de/sites/default/files/election-program-files/vorlaufigmieterparteiwahlprogrammltwbln2023.pdf</t>
+  </si>
+  <si>
+    <t>https://www.abgeordnetenwatch.de/sites/default/files/election-program-files/odpparteiprogramm.pdf</t>
+  </si>
+  <si>
+    <t>https://www.abgeordnetenwatch.de/sites/default/files/election-program-files/gesundheitsforschungwahlprogramm.pdf</t>
+  </si>
+  <si>
+    <t>https://www.abgeordnetenwatch.de/sites/default/files/election-program-files/piraten-wp-agh-2021.pdf</t>
+  </si>
+  <si>
+    <t>https://www.abgeordnetenwatch.de/sites/default/files/election-program-files/graue-pantherwahlaufruf.pdf</t>
+  </si>
+  <si>
+    <t>Graue</t>
+  </si>
+  <si>
+    <t>SGP</t>
+  </si>
+  <si>
+    <t>https://www.abgeordnetenwatch.de/sites/default/files/election-program-files/sgpwahlaufruf.pdf</t>
+  </si>
+  <si>
+    <t>Todenhöfer</t>
+  </si>
+  <si>
+    <t>https://www.abgeordnetenwatch.de/sites/default/files/election-program-files/teamtodenhoferwahlprogramm.pdf</t>
+  </si>
+  <si>
+    <t>https://www.abgeordnetenwatch.de/sites/default/files/election-program-files/voltwahlprogrammltwbln2023.pdf</t>
   </si>
 </sst>
 </file>
@@ -1536,11 +1647,11 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:E314"/>
+  <dimension ref="A1:E341"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A281" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E317" sqref="E317"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A340" sqref="A340"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
@@ -6889,7 +7000,467 @@
         <v>397</v>
       </c>
     </row>
+    <row r="315" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A315" t="s">
+        <v>48</v>
+      </c>
+      <c r="B315">
+        <v>2023</v>
+      </c>
+      <c r="C315" t="s">
+        <v>6</v>
+      </c>
+      <c r="D315" t="s">
+        <v>7</v>
+      </c>
+      <c r="E315" t="s">
+        <v>402</v>
+      </c>
+    </row>
+    <row r="316" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A316" t="s">
+        <v>48</v>
+      </c>
+      <c r="B316">
+        <v>2023</v>
+      </c>
+      <c r="C316" t="s">
+        <v>9</v>
+      </c>
+      <c r="D316" t="s">
+        <v>7</v>
+      </c>
+      <c r="E316" t="s">
+        <v>400</v>
+      </c>
+    </row>
+    <row r="317" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A317" t="s">
+        <v>48</v>
+      </c>
+      <c r="B317">
+        <v>2023</v>
+      </c>
+      <c r="C317" t="s">
+        <v>11</v>
+      </c>
+      <c r="D317" t="s">
+        <v>7</v>
+      </c>
+      <c r="E317" t="s">
+        <v>399</v>
+      </c>
+    </row>
+    <row r="318" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A318" t="s">
+        <v>48</v>
+      </c>
+      <c r="B318">
+        <v>2023</v>
+      </c>
+      <c r="C318" t="s">
+        <v>25</v>
+      </c>
+      <c r="D318" t="s">
+        <v>7</v>
+      </c>
+      <c r="E318" t="s">
+        <v>413</v>
+      </c>
+    </row>
+    <row r="319" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A319" t="s">
+        <v>48</v>
+      </c>
+      <c r="B319">
+        <v>2023</v>
+      </c>
+      <c r="C319" t="s">
+        <v>32</v>
+      </c>
+      <c r="D319" t="s">
+        <v>7</v>
+      </c>
+      <c r="E319" t="s">
+        <v>401</v>
+      </c>
+    </row>
+    <row r="320" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A320" t="s">
+        <v>48</v>
+      </c>
+      <c r="B320">
+        <v>2023</v>
+      </c>
+      <c r="C320" t="s">
+        <v>26</v>
+      </c>
+      <c r="D320" t="s">
+        <v>7</v>
+      </c>
+      <c r="E320" t="s">
+        <v>419</v>
+      </c>
+    </row>
+    <row r="321" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A321" t="s">
+        <v>48</v>
+      </c>
+      <c r="B321">
+        <v>2023</v>
+      </c>
+      <c r="C321" t="s">
+        <v>27</v>
+      </c>
+      <c r="D321" t="s">
+        <v>7</v>
+      </c>
+      <c r="E321" t="s">
+        <v>403</v>
+      </c>
+    </row>
+    <row r="322" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A322" t="s">
+        <v>48</v>
+      </c>
+      <c r="B322">
+        <v>2023</v>
+      </c>
+      <c r="C322" t="s">
+        <v>97</v>
+      </c>
+      <c r="D322" t="s">
+        <v>7</v>
+      </c>
+      <c r="E322" t="s">
+        <v>420</v>
+      </c>
+    </row>
+    <row r="323" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A323" t="s">
+        <v>48</v>
+      </c>
+      <c r="B323">
+        <v>2023</v>
+      </c>
+      <c r="C323" t="s">
+        <v>28</v>
+      </c>
+      <c r="D323" t="s">
+        <v>7</v>
+      </c>
+      <c r="E323" t="s">
+        <v>421</v>
+      </c>
+    </row>
+    <row r="324" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A324" t="s">
+        <v>48</v>
+      </c>
+      <c r="B324">
+        <v>2023</v>
+      </c>
+      <c r="C324" t="s">
+        <v>82</v>
+      </c>
+      <c r="D324" t="s">
+        <v>7</v>
+      </c>
+      <c r="E324" t="s">
+        <v>424</v>
+      </c>
+    </row>
+    <row r="325" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A325" t="s">
+        <v>48</v>
+      </c>
+      <c r="B325">
+        <v>2023</v>
+      </c>
+      <c r="C325" t="s">
+        <v>29</v>
+      </c>
+      <c r="D325" t="s">
+        <v>7</v>
+      </c>
+      <c r="E325" t="s">
+        <v>425</v>
+      </c>
+    </row>
+    <row r="326" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A326" t="s">
+        <v>48</v>
+      </c>
+      <c r="B326">
+        <v>2023</v>
+      </c>
+      <c r="C326" t="s">
+        <v>30</v>
+      </c>
+      <c r="D326" t="s">
+        <v>7</v>
+      </c>
+      <c r="E326" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="327" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A327" t="s">
+        <v>48</v>
+      </c>
+      <c r="B327">
+        <v>2023</v>
+      </c>
+      <c r="C327" t="s">
+        <v>31</v>
+      </c>
+      <c r="D327" t="s">
+        <v>7</v>
+      </c>
+      <c r="E327" t="s">
+        <v>434</v>
+      </c>
+    </row>
+    <row r="328" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A328" t="s">
+        <v>48</v>
+      </c>
+      <c r="B328">
+        <v>2023</v>
+      </c>
+      <c r="C328" t="s">
+        <v>405</v>
+      </c>
+      <c r="D328" t="s">
+        <v>7</v>
+      </c>
+      <c r="E328" t="s">
+        <v>404</v>
+      </c>
+    </row>
+    <row r="329" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A329" t="s">
+        <v>48</v>
+      </c>
+      <c r="B329">
+        <v>2023</v>
+      </c>
+      <c r="C329" t="s">
+        <v>407</v>
+      </c>
+      <c r="D329" t="s">
+        <v>70</v>
+      </c>
+      <c r="E329" t="s">
+        <v>406</v>
+      </c>
+    </row>
+    <row r="330" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A330" t="s">
+        <v>48</v>
+      </c>
+      <c r="B330">
+        <v>2023</v>
+      </c>
+      <c r="C330" t="s">
+        <v>409</v>
+      </c>
+      <c r="D330" t="s">
+        <v>70</v>
+      </c>
+      <c r="E330" t="s">
+        <v>408</v>
+      </c>
+    </row>
+    <row r="331" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A331" t="s">
+        <v>48</v>
+      </c>
+      <c r="B331">
+        <v>2023</v>
+      </c>
+      <c r="C331" t="s">
+        <v>411</v>
+      </c>
+      <c r="D331" t="s">
+        <v>70</v>
+      </c>
+      <c r="E331" t="s">
+        <v>410</v>
+      </c>
+    </row>
+    <row r="332" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A332" t="s">
+        <v>48</v>
+      </c>
+      <c r="B332">
+        <v>2023</v>
+      </c>
+      <c r="C332" t="s">
+        <v>348</v>
+      </c>
+      <c r="D332" t="s">
+        <v>7</v>
+      </c>
+      <c r="E332" t="s">
+        <v>412</v>
+      </c>
+    </row>
+    <row r="333" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A333" t="s">
+        <v>48</v>
+      </c>
+      <c r="B333">
+        <v>2023</v>
+      </c>
+      <c r="C333" t="s">
+        <v>414</v>
+      </c>
+      <c r="D333" t="s">
+        <v>70</v>
+      </c>
+      <c r="E333" t="s">
+        <v>415</v>
+      </c>
+    </row>
+    <row r="334" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A334" t="s">
+        <v>48</v>
+      </c>
+      <c r="B334">
+        <v>2023</v>
+      </c>
+      <c r="C334" t="s">
+        <v>80</v>
+      </c>
+      <c r="D334" t="s">
+        <v>7</v>
+      </c>
+      <c r="E334" t="s">
+        <v>416</v>
+      </c>
+    </row>
+    <row r="335" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A335" t="s">
+        <v>48</v>
+      </c>
+      <c r="B335">
+        <v>2023</v>
+      </c>
+      <c r="C335" t="s">
+        <v>418</v>
+      </c>
+      <c r="D335" t="s">
+        <v>7</v>
+      </c>
+      <c r="E335" t="s">
+        <v>417</v>
+      </c>
+    </row>
+    <row r="336" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A336" t="s">
+        <v>48</v>
+      </c>
+      <c r="B336">
+        <v>2023</v>
+      </c>
+      <c r="C336" t="s">
+        <v>423</v>
+      </c>
+      <c r="D336" t="s">
+        <v>70</v>
+      </c>
+      <c r="E336" t="s">
+        <v>422</v>
+      </c>
+    </row>
+    <row r="337" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A337" t="s">
+        <v>48</v>
+      </c>
+      <c r="B337">
+        <v>2023</v>
+      </c>
+      <c r="C337" t="s">
+        <v>67</v>
+      </c>
+      <c r="D337" t="s">
+        <v>7</v>
+      </c>
+      <c r="E337" t="s">
+        <v>426</v>
+      </c>
+    </row>
+    <row r="338" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A338" t="s">
+        <v>48</v>
+      </c>
+      <c r="B338">
+        <v>2023</v>
+      </c>
+      <c r="C338" t="s">
+        <v>34</v>
+      </c>
+      <c r="D338" t="s">
+        <v>7</v>
+      </c>
+      <c r="E338" t="s">
+        <v>427</v>
+      </c>
+    </row>
+    <row r="339" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A339" t="s">
+        <v>48</v>
+      </c>
+      <c r="B339">
+        <v>2023</v>
+      </c>
+      <c r="C339" t="s">
+        <v>429</v>
+      </c>
+      <c r="D339" t="s">
+        <v>7</v>
+      </c>
+      <c r="E339" t="s">
+        <v>428</v>
+      </c>
+    </row>
+    <row r="340" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A340" t="s">
+        <v>48</v>
+      </c>
+      <c r="B340">
+        <v>2023</v>
+      </c>
+      <c r="C340" t="s">
+        <v>430</v>
+      </c>
+      <c r="D340" t="s">
+        <v>7</v>
+      </c>
+      <c r="E340" t="s">
+        <v>431</v>
+      </c>
+    </row>
+    <row r="341" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A341" t="s">
+        <v>48</v>
+      </c>
+      <c r="B341">
+        <v>2023</v>
+      </c>
+      <c r="C341" t="s">
+        <v>432</v>
+      </c>
+      <c r="D341" t="s">
+        <v>70</v>
+      </c>
+      <c r="E341" t="s">
+        <v>433</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
 </worksheet>
 </file>
</xml_diff>